<commit_message>
feat(Productos - Metadatos): Agregado campo de detalles técnicos
</commit_message>
<xml_diff>
--- a/archivos/plantillas/productos_metadatos.xlsx
+++ b/archivos/plantillas/productos_metadatos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\proyectos\simon-bolivar\application\views\reportes\plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\proyectos\simon-bolivar\archivos\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B4165F-F74F-4513-852E-0E7A5291C70A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F54CCF9-83EE-4E33-9104-42C0AD4075F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="21060" windowHeight="15585" xr2:uid="{3ADC2AB6-8EEB-4A74-A297-568E13D56A3F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3ADC2AB6-8EEB-4A74-A297-568E13D56A3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>URL</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>https://repuestossimonbolivar.com/productos/ver/buje-balancin-trailer</t>
+  </si>
+  <si>
+    <t>detalles técnicos</t>
+  </si>
+  <si>
+    <t>Valores técnicos</t>
   </si>
 </sst>
 </file>
@@ -162,34 +168,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -526,21 +523,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD43C620-A685-4D48-BB84-C9191162DE12}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="69.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.85546875" style="9" customWidth="1"/>
-    <col min="5" max="5" width="78.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="9"/>
+    <col min="1" max="1" width="51" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" style="6" customWidth="1"/>
+    <col min="4" max="5" width="41.28515625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="66.42578125" style="6" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -550,33 +549,39 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{95026E66-2742-4EA4-931F-90D7670BAAB4}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{95026E66-2742-4EA4-931F-90D7670BAAB4}"/>
     <hyperlink ref="A2" r:id="rId2" xr:uid="{9E573F2C-C5B3-4FB4-9FFB-BB9CFCB4671D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>